<commit_message>
Korrektur før første publisering v22
</commit_message>
<xml_diff>
--- a/tidligere-eksamensoppgaver/hjemmeeksamen.xlsx
+++ b/tidligere-eksamensoppgaver/hjemmeeksamen.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s14363\Documents\temp2\met4\tidligere-eksamensoppgaver\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hakon\repositories\met4\tidligere-eksamensoppgaver\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D34C336C-D34A-4219-99CF-7E43E22C584E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8ABFB83-BD3F-466F-A5B0-64139D6A74FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17790" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
   <si>
     <t>Semester</t>
   </si>
@@ -145,6 +145,18 @@
   </si>
   <si>
     <t>Data ikke lenger tilgjengelig.</t>
+  </si>
+  <si>
+    <t>2021 - Høst</t>
+  </si>
+  <si>
+    <t>[Oppgaveformulering](tidligere-eksamensoppgaver/hjemme-21-h.pdf)</t>
+  </si>
+  <si>
+    <t>[Materiale](tidligere-eksamensoppgaver/hjemme-21-h-ekstra.zip)</t>
+  </si>
+  <si>
+    <t>[Løsningsforslag](tidligere-eksamensoppgaver/hjemme-21-h-solprop.html)</t>
   </si>
 </sst>
 </file>
@@ -462,10 +474,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -616,6 +628,20 @@
         <v>39</v>
       </c>
     </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>40</v>
+      </c>
+      <c r="B11" t="s">
+        <v>41</v>
+      </c>
+      <c r="C11" t="s">
+        <v>43</v>
+      </c>
+      <c r="D11" t="s">
+        <v>42</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
fikset død link heks v22
</commit_message>
<xml_diff>
--- a/tidligere-eksamensoppgaver/hjemmeeksamen.xlsx
+++ b/tidligere-eksamensoppgaver/hjemmeeksamen.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s12203\repos\met4\tidligere-eksamensoppgaver\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{154AD14C-E706-455B-B5A2-B93F20491ED4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8562FEA-2285-48FA-A8AB-C04388ABAACD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-195" windowWidth="29040" windowHeight="17790" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -171,9 +171,6 @@
     <t>[Oppgaveformulering](tidligere-eksamensoppgaver/hjemme-22-h.pdf)</t>
   </si>
   <si>
-    <t>[Løsningsforslag](tidligere-eksamensoppgaver/hjemme-22-v-solprop.pdf)</t>
-  </si>
-  <si>
     <t>[Løsningsforslag](tidligere-eksamensoppgaver/hjemme-22-h-solprop.html)</t>
   </si>
   <si>
@@ -181,6 +178,9 @@
   </si>
   <si>
     <t>[Materiale](tidligere-eksamensoppgaver/hjemme-22-h-ekstra.zip)</t>
+  </si>
+  <si>
+    <t>[Løsningsforslag](tidligere-eksamensoppgaver/hjemme-22-v-solprop.html)</t>
   </si>
 </sst>
 </file>
@@ -501,7 +501,7 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -674,10 +674,10 @@
         <v>46</v>
       </c>
       <c r="C12" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="D12" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -688,10 +688,10 @@
         <v>47</v>
       </c>
       <c r="C13" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D13" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Oppdatert til vår 2023
</commit_message>
<xml_diff>
--- a/tidligere-eksamensoppgaver/hjemmeeksamen.xlsx
+++ b/tidligere-eksamensoppgaver/hjemmeeksamen.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s14363\Documents\met4git\met4\tidligere-eksamensoppgaver\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\met4\tidligere-eksamensoppgaver\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3133B6E-7F6A-4F48-8D76-9C006FD96FCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11DE9142-0F97-4FA0-ABA0-22598359446F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="60">
   <si>
     <t>Semester</t>
   </si>
@@ -193,6 +193,18 @@
   </si>
   <si>
     <t>[Materiale](tidligere-eksamensoppgaver/hjemme-23-v-ekstra.zip)</t>
+  </si>
+  <si>
+    <t>2023 - Høst</t>
+  </si>
+  <si>
+    <t>[Oppgaveformulering](tidligere-eksamensoppgaver/hjemme-23-h.pdf)</t>
+  </si>
+  <si>
+    <t>[Løsningsforslag](tidligere-eksamensoppgaver/hjemme-23-h-solprop.html)</t>
+  </si>
+  <si>
+    <t>[Materiale](tidligere-eksamensoppgaver/hjemme-23-h-ekstra.zip)</t>
   </si>
 </sst>
 </file>
@@ -510,21 +522,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="19" customWidth="1"/>
-    <col min="2" max="2" width="52.33203125" customWidth="1"/>
-    <col min="3" max="3" width="66.109375" customWidth="1"/>
-    <col min="4" max="4" width="57.6640625" customWidth="1"/>
+    <col min="2" max="2" width="52.36328125" customWidth="1"/>
+    <col min="3" max="3" width="66.08984375" customWidth="1"/>
+    <col min="4" max="4" width="57.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -538,7 +550,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -552,7 +564,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -566,7 +578,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -580,7 +592,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -594,7 +606,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -608,7 +620,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -622,7 +634,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -636,7 +648,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -650,7 +662,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>36</v>
       </c>
@@ -664,7 +676,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>40</v>
       </c>
@@ -678,7 +690,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>44</v>
       </c>
@@ -692,7 +704,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>45</v>
       </c>
@@ -706,7 +718,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>52</v>
       </c>
@@ -718,6 +730,20 @@
       </c>
       <c r="D14" t="s">
         <v>55</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>56</v>
+      </c>
+      <c r="B15" t="s">
+        <v>57</v>
+      </c>
+      <c r="C15" t="s">
+        <v>58</v>
+      </c>
+      <c r="D15" t="s">
+        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>